<commit_message>
minor bug fixes and reformating code
moveport are changed into counting system for easier TL movement. 
cleaning moving port
minor fixes on port names 'P. ' into 'P.' also ' / ' and other spacing variables into '/' 
deleting some double port names
some update on port movement
</commit_message>
<xml_diff>
--- a/Data Integrasi.xlsx
+++ b/Data Integrasi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\Freelancing\Genetic Algorithm Jaringan Kapal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\Freelancing\Genetic Algorithm Jaringan Kapal\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0527A4D9-4DD6-42FA-BEF3-E8778734D81B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2D78B0-92D4-4464-8766-412467F8B2A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="845" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5289,22 +5289,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
     <mergeCell ref="I16:I17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:H49"/>
     <mergeCell ref="I48:I49"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="E23:E24"/>
@@ -5313,6 +5305,14 @@
     <mergeCell ref="H37:H38"/>
     <mergeCell ref="I37:I38"/>
     <mergeCell ref="G31:G32"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="G23:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
@@ -15575,8 +15575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:O54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L57" sqref="L57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FINISH THE DAMN MOVING STORAGE PROBLEM
ALWAYS REMOVE STUPID WHITESPACES YOU IDIOT
</commit_message>
<xml_diff>
--- a/Data Integrasi.xlsx
+++ b/Data Integrasi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\Freelancing\Genetic Algorithm Jaringan Kapal\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2D78B0-92D4-4464-8766-412467F8B2A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B502B7B4-C9DC-493A-B605-17E340C7CCCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="845" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="20490" windowHeight="10905" tabRatio="845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tol Laut" sheetId="6" r:id="rId1"/>
@@ -1111,20 +1111,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1138,10 +1138,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4387,8 +4387,8 @@
   </sheetPr>
   <dimension ref="A2:O62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4515,22 +4515,22 @@
       <c r="C16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="64" t="s">
+      <c r="D16" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="64" t="s">
+      <c r="E16" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="64" t="s">
+      <c r="G16" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="66" t="s">
+      <c r="H16" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="I16" s="64" t="s">
+      <c r="I16" s="66" t="s">
         <v>9</v>
       </c>
       <c r="J16" s="7"/>
@@ -4539,12 +4539,12 @@
       <c r="C17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
       <c r="F17" s="65"/>
       <c r="G17" s="65"/>
       <c r="H17" s="65"/>
-      <c r="I17" s="64"/>
+      <c r="I17" s="66"/>
       <c r="J17" s="7"/>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
@@ -4614,22 +4614,22 @@
       <c r="C23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="64" t="s">
+      <c r="D23" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="E23" s="64" t="s">
+      <c r="E23" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="64" t="s">
+      <c r="F23" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="64" t="s">
+      <c r="G23" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="66" t="s">
+      <c r="H23" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="I23" s="64" t="s">
+      <c r="I23" s="66" t="s">
         <v>9</v>
       </c>
       <c r="K23" s="17"/>
@@ -4642,12 +4642,12 @@
       <c r="C24" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
       <c r="F24" s="65"/>
       <c r="G24" s="65"/>
       <c r="H24" s="65"/>
-      <c r="I24" s="64"/>
+      <c r="I24" s="66"/>
       <c r="K24" s="17"/>
       <c r="L24" s="17"/>
       <c r="M24" s="17"/>
@@ -4745,13 +4745,13 @@
       <c r="F31" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="66" t="s">
+      <c r="G31" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="66" t="s">
+      <c r="H31" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="I31" s="66" t="s">
+      <c r="I31" s="64" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4851,13 +4851,13 @@
       <c r="F37" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="G37" s="66" t="s">
+      <c r="G37" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="H37" s="66" t="s">
+      <c r="H37" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="I37" s="66" t="s">
+      <c r="I37" s="64" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5031,33 +5031,33 @@
       <c r="C48" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="64" t="s">
+      <c r="D48" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="E48" s="64" t="s">
+      <c r="E48" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="F48" s="64" t="s">
+      <c r="F48" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="G48" s="64" t="s">
+      <c r="G48" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="H48" s="66" t="s">
+      <c r="H48" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="I48" s="64" t="s">
+      <c r="I48" s="66" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="49" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C49" s="3"/>
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="66"/>
       <c r="F49" s="65"/>
       <c r="G49" s="65"/>
       <c r="H49" s="65"/>
-      <c r="I49" s="64"/>
+      <c r="I49" s="66"/>
     </row>
     <row r="50" spans="3:10" s="46" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="57" t="s">
@@ -5289,14 +5289,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
     <mergeCell ref="I48:I49"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="E23:E24"/>
@@ -5313,6 +5305,14 @@
     <mergeCell ref="H31:H32"/>
     <mergeCell ref="I31:I32"/>
     <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
@@ -5375,19 +5375,19 @@
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="66" t="s">
+      <c r="D7" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="66" t="s">
+      <c r="F7" s="64" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="67" t="s">
+      <c r="H7" s="68" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5399,7 +5399,7 @@
       <c r="E8" s="65"/>
       <c r="F8" s="65"/>
       <c r="G8" s="70"/>
-      <c r="H8" s="67"/>
+      <c r="H8" s="68"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
@@ -5496,10 +5496,10 @@
       <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="68" t="s">
+      <c r="D14" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="68" t="s">
+      <c r="E14" s="67" t="s">
         <v>3</v>
       </c>
       <c r="F14" s="13"/>
@@ -5512,8 +5512,8 @@
       <c r="C15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
@@ -5571,25 +5571,25 @@
       <c r="C22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="68" t="s">
+      <c r="D22" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="68" t="s">
+      <c r="E22" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="64" t="s">
+      <c r="G22" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="64" t="s">
+      <c r="H22" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="I22" s="67" t="s">
+      <c r="I22" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J22" s="67" t="s">
+      <c r="J22" s="68" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5597,13 +5597,13 @@
       <c r="C23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
@@ -5731,25 +5731,25 @@
       <c r="C30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="68" t="s">
+      <c r="D30" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="68" t="s">
+      <c r="E30" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="64" t="s">
+      <c r="F30" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="64" t="s">
+      <c r="G30" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="H30" s="64" t="s">
+      <c r="H30" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="I30" s="67" t="s">
+      <c r="I30" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J30" s="67" t="s">
+      <c r="J30" s="68" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5757,13 +5757,13 @@
       <c r="C31" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="67"/>
-      <c r="J31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C32" s="4" t="s">
@@ -6007,37 +6007,37 @@
       <c r="C43" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="68" t="s">
+      <c r="D43" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="68" t="s">
+      <c r="E43" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="64" t="s">
+      <c r="F43" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="G43" s="64" t="s">
+      <c r="G43" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="H43" s="64" t="s">
+      <c r="H43" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="67" t="s">
+      <c r="I43" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J43" s="67" t="s">
+      <c r="J43" s="68" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C44" s="3"/>
-      <c r="D44" s="68"/>
-      <c r="E44" s="68"/>
-      <c r="F44" s="64"/>
-      <c r="G44" s="64"/>
-      <c r="H44" s="64"/>
-      <c r="I44" s="67"/>
-      <c r="J44" s="67"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="66"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="68"/>
+      <c r="J44" s="68"/>
     </row>
     <row r="45" spans="3:11" s="46" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C45" s="57" t="s">
@@ -6408,23 +6408,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
     <mergeCell ref="I43:I44"/>
     <mergeCell ref="J43:J44"/>
     <mergeCell ref="F22:F23"/>
@@ -6436,6 +6419,23 @@
     <mergeCell ref="H30:H31"/>
     <mergeCell ref="I22:I23"/>
     <mergeCell ref="J22:J23"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
@@ -6571,19 +6571,19 @@
       <c r="W11" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="X11" s="73" t="s">
+      <c r="X11" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="Y11" s="73" t="s">
+      <c r="Y11" s="74" t="s">
         <v>13</v>
       </c>
       <c r="Z11" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="AA11" s="73" t="s">
+      <c r="AA11" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="AB11" s="73" t="s">
+      <c r="AB11" s="74" t="s">
         <v>14</v>
       </c>
       <c r="AC11" s="71" t="s">
@@ -6601,16 +6601,16 @@
       <c r="AG11" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="AH11" s="73" t="s">
+      <c r="AH11" s="74" t="s">
         <v>72</v>
       </c>
       <c r="AI11" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="AJ11" s="73" t="s">
+      <c r="AJ11" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="AK11" s="73" t="s">
+      <c r="AK11" s="74" t="s">
         <v>71</v>
       </c>
       <c r="AL11" s="71" t="s">
@@ -6734,32 +6734,32 @@
       <c r="I12" s="72"/>
       <c r="J12" s="72"/>
       <c r="K12" s="72"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
-      <c r="N12" s="74"/>
-      <c r="O12" s="74"/>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="74"/>
-      <c r="T12" s="74"/>
-      <c r="U12" s="74"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="73"/>
+      <c r="R12" s="73"/>
+      <c r="S12" s="73"/>
+      <c r="T12" s="73"/>
+      <c r="U12" s="73"/>
       <c r="V12" s="72"/>
       <c r="W12" s="72"/>
-      <c r="X12" s="73"/>
-      <c r="Y12" s="73"/>
+      <c r="X12" s="74"/>
+      <c r="Y12" s="74"/>
       <c r="Z12" s="72"/>
-      <c r="AA12" s="73"/>
-      <c r="AB12" s="73"/>
+      <c r="AA12" s="74"/>
+      <c r="AB12" s="74"/>
       <c r="AC12" s="72"/>
       <c r="AD12" s="72"/>
       <c r="AE12" s="72"/>
       <c r="AF12" s="72"/>
       <c r="AG12" s="72"/>
-      <c r="AH12" s="73"/>
+      <c r="AH12" s="74"/>
       <c r="AI12" s="72"/>
-      <c r="AJ12" s="73"/>
-      <c r="AK12" s="73"/>
+      <c r="AJ12" s="74"/>
+      <c r="AK12" s="74"/>
       <c r="AL12" s="72"/>
       <c r="AM12" s="72"/>
       <c r="AN12" s="72"/>
@@ -7893,19 +7893,19 @@
       <c r="W25" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="X25" s="73" t="s">
+      <c r="X25" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="Y25" s="73" t="s">
+      <c r="Y25" s="74" t="s">
         <v>13</v>
       </c>
       <c r="Z25" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="AA25" s="73" t="s">
+      <c r="AA25" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="AB25" s="73" t="s">
+      <c r="AB25" s="74" t="s">
         <v>14</v>
       </c>
       <c r="AC25" s="71" t="s">
@@ -7923,16 +7923,16 @@
       <c r="AG25" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="AH25" s="73" t="s">
+      <c r="AH25" s="74" t="s">
         <v>72</v>
       </c>
       <c r="AI25" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="AJ25" s="73" t="s">
+      <c r="AJ25" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="AK25" s="73" t="s">
+      <c r="AK25" s="74" t="s">
         <v>71</v>
       </c>
       <c r="AL25" s="71" t="s">
@@ -8068,20 +8068,20 @@
       <c r="U26" s="72"/>
       <c r="V26" s="72"/>
       <c r="W26" s="72"/>
-      <c r="X26" s="73"/>
-      <c r="Y26" s="73"/>
+      <c r="X26" s="74"/>
+      <c r="Y26" s="74"/>
       <c r="Z26" s="72"/>
-      <c r="AA26" s="73"/>
-      <c r="AB26" s="73"/>
+      <c r="AA26" s="74"/>
+      <c r="AB26" s="74"/>
       <c r="AC26" s="72"/>
       <c r="AD26" s="72"/>
       <c r="AE26" s="72"/>
       <c r="AF26" s="72"/>
       <c r="AG26" s="72"/>
-      <c r="AH26" s="73"/>
+      <c r="AH26" s="74"/>
       <c r="AI26" s="72"/>
-      <c r="AJ26" s="73"/>
-      <c r="AK26" s="73"/>
+      <c r="AJ26" s="74"/>
+      <c r="AK26" s="74"/>
       <c r="AL26" s="72"/>
       <c r="AM26" s="72"/>
       <c r="AN26" s="72"/>
@@ -10807,19 +10807,19 @@
       <c r="W38" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="X38" s="73" t="s">
+      <c r="X38" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="Y38" s="73" t="s">
+      <c r="Y38" s="74" t="s">
         <v>13</v>
       </c>
       <c r="Z38" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="AA38" s="73" t="s">
+      <c r="AA38" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="AB38" s="73" t="s">
+      <c r="AB38" s="74" t="s">
         <v>14</v>
       </c>
       <c r="AC38" s="71" t="s">
@@ -10837,16 +10837,16 @@
       <c r="AG38" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="AH38" s="73" t="s">
+      <c r="AH38" s="74" t="s">
         <v>72</v>
       </c>
       <c r="AI38" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="AJ38" s="73" t="s">
+      <c r="AJ38" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="AK38" s="73" t="s">
+      <c r="AK38" s="74" t="s">
         <v>71</v>
       </c>
       <c r="AL38" s="71" t="s">
@@ -10982,20 +10982,20 @@
       <c r="U39" s="72"/>
       <c r="V39" s="72"/>
       <c r="W39" s="72"/>
-      <c r="X39" s="73"/>
-      <c r="Y39" s="73"/>
+      <c r="X39" s="74"/>
+      <c r="Y39" s="74"/>
       <c r="Z39" s="72"/>
-      <c r="AA39" s="73"/>
-      <c r="AB39" s="73"/>
+      <c r="AA39" s="74"/>
+      <c r="AB39" s="74"/>
       <c r="AC39" s="72"/>
       <c r="AD39" s="72"/>
       <c r="AE39" s="72"/>
       <c r="AF39" s="72"/>
       <c r="AG39" s="72"/>
-      <c r="AH39" s="73"/>
+      <c r="AH39" s="74"/>
       <c r="AI39" s="72"/>
-      <c r="AJ39" s="73"/>
-      <c r="AK39" s="73"/>
+      <c r="AJ39" s="74"/>
+      <c r="AK39" s="74"/>
       <c r="AL39" s="72"/>
       <c r="AM39" s="72"/>
       <c r="AN39" s="72"/>
@@ -13064,19 +13064,19 @@
       <c r="W52" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="X52" s="73" t="s">
+      <c r="X52" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="Y52" s="73" t="s">
+      <c r="Y52" s="74" t="s">
         <v>13</v>
       </c>
       <c r="Z52" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="AA52" s="73" t="s">
+      <c r="AA52" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="AB52" s="73" t="s">
+      <c r="AB52" s="74" t="s">
         <v>14</v>
       </c>
       <c r="AC52" s="71" t="s">
@@ -13094,16 +13094,16 @@
       <c r="AG52" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="AH52" s="73" t="s">
+      <c r="AH52" s="74" t="s">
         <v>72</v>
       </c>
       <c r="AI52" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="AJ52" s="73" t="s">
+      <c r="AJ52" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="AK52" s="73" t="s">
+      <c r="AK52" s="74" t="s">
         <v>71</v>
       </c>
       <c r="AL52" s="71" t="s">
@@ -13237,20 +13237,20 @@
       <c r="U53" s="72"/>
       <c r="V53" s="72"/>
       <c r="W53" s="72"/>
-      <c r="X53" s="73"/>
-      <c r="Y53" s="73"/>
+      <c r="X53" s="74"/>
+      <c r="Y53" s="74"/>
       <c r="Z53" s="72"/>
-      <c r="AA53" s="73"/>
-      <c r="AB53" s="73"/>
+      <c r="AA53" s="74"/>
+      <c r="AB53" s="74"/>
       <c r="AC53" s="72"/>
       <c r="AD53" s="72"/>
       <c r="AE53" s="72"/>
       <c r="AF53" s="72"/>
       <c r="AG53" s="72"/>
-      <c r="AH53" s="73"/>
+      <c r="AH53" s="74"/>
       <c r="AI53" s="72"/>
-      <c r="AJ53" s="73"/>
-      <c r="AK53" s="73"/>
+      <c r="AJ53" s="74"/>
+      <c r="AK53" s="74"/>
       <c r="AL53" s="72"/>
       <c r="AM53" s="72"/>
       <c r="AN53" s="72"/>
@@ -15254,6 +15254,262 @@
     </row>
   </sheetData>
   <mergeCells count="280">
+    <mergeCell ref="BO52:BO53"/>
+    <mergeCell ref="T52:T53"/>
+    <mergeCell ref="S52:S53"/>
+    <mergeCell ref="V52:V53"/>
+    <mergeCell ref="X52:X53"/>
+    <mergeCell ref="AT52:AT53"/>
+    <mergeCell ref="AU52:AU53"/>
+    <mergeCell ref="BA52:BA53"/>
+    <mergeCell ref="BF52:BF53"/>
+    <mergeCell ref="AY52:AY53"/>
+    <mergeCell ref="AZ52:AZ53"/>
+    <mergeCell ref="AI52:AI53"/>
+    <mergeCell ref="BC52:BC53"/>
+    <mergeCell ref="BD52:BD53"/>
+    <mergeCell ref="AR52:AR53"/>
+    <mergeCell ref="BG52:BG53"/>
+    <mergeCell ref="BH52:BH53"/>
+    <mergeCell ref="W52:W53"/>
+    <mergeCell ref="BS52:BS53"/>
+    <mergeCell ref="BT52:BT53"/>
+    <mergeCell ref="BU52:BU53"/>
+    <mergeCell ref="AW52:AW53"/>
+    <mergeCell ref="AG52:AG53"/>
+    <mergeCell ref="AD52:AD53"/>
+    <mergeCell ref="AC52:AC53"/>
+    <mergeCell ref="AE52:AE53"/>
+    <mergeCell ref="AB52:AB53"/>
+    <mergeCell ref="AJ52:AJ53"/>
+    <mergeCell ref="AK52:AK53"/>
+    <mergeCell ref="AH52:AH53"/>
+    <mergeCell ref="BR52:BR53"/>
+    <mergeCell ref="BQ52:BQ53"/>
+    <mergeCell ref="BP52:BP53"/>
+    <mergeCell ref="BE52:BE53"/>
+    <mergeCell ref="BL52:BL53"/>
+    <mergeCell ref="BM52:BM53"/>
+    <mergeCell ref="AS52:AS53"/>
+    <mergeCell ref="BI52:BI53"/>
+    <mergeCell ref="BJ52:BJ53"/>
+    <mergeCell ref="BK52:BK53"/>
+    <mergeCell ref="BB52:BB53"/>
+    <mergeCell ref="BN52:BN53"/>
+    <mergeCell ref="R52:R53"/>
+    <mergeCell ref="AX52:AX53"/>
+    <mergeCell ref="O52:O53"/>
+    <mergeCell ref="P52:P53"/>
+    <mergeCell ref="Q52:Q53"/>
+    <mergeCell ref="AF52:AF53"/>
+    <mergeCell ref="M52:M53"/>
+    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="AL52:AL53"/>
+    <mergeCell ref="AV52:AV53"/>
+    <mergeCell ref="U52:U53"/>
+    <mergeCell ref="AO52:AO53"/>
+    <mergeCell ref="AP52:AP53"/>
+    <mergeCell ref="AQ52:AQ53"/>
+    <mergeCell ref="Y52:Y53"/>
+    <mergeCell ref="AA52:AA53"/>
+    <mergeCell ref="AM52:AM53"/>
+    <mergeCell ref="AN52:AN53"/>
+    <mergeCell ref="Z52:Z53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="H52:H53"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="K52:K53"/>
+    <mergeCell ref="L52:L53"/>
+    <mergeCell ref="W38:W39"/>
+    <mergeCell ref="R38:R39"/>
+    <mergeCell ref="AX38:AX39"/>
+    <mergeCell ref="AY38:AY39"/>
+    <mergeCell ref="AZ38:AZ39"/>
+    <mergeCell ref="AT38:AT39"/>
+    <mergeCell ref="BC38:BC39"/>
+    <mergeCell ref="BD38:BD39"/>
+    <mergeCell ref="AR38:AR39"/>
+    <mergeCell ref="AS38:AS39"/>
+    <mergeCell ref="AW38:AW39"/>
+    <mergeCell ref="Z38:Z39"/>
+    <mergeCell ref="AE38:AE39"/>
+    <mergeCell ref="AB38:AB39"/>
+    <mergeCell ref="AJ38:AJ39"/>
+    <mergeCell ref="AK38:AK39"/>
+    <mergeCell ref="AH38:AH39"/>
+    <mergeCell ref="AI38:AI39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="S38:S39"/>
+    <mergeCell ref="BK38:BK39"/>
+    <mergeCell ref="BS38:BS39"/>
+    <mergeCell ref="P38:P39"/>
+    <mergeCell ref="Q38:Q39"/>
+    <mergeCell ref="AF38:AF39"/>
+    <mergeCell ref="AG38:AG39"/>
+    <mergeCell ref="AD38:AD39"/>
+    <mergeCell ref="AC38:AC39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="O38:O39"/>
+    <mergeCell ref="BM38:BM39"/>
+    <mergeCell ref="BB38:BB39"/>
+    <mergeCell ref="BN38:BN39"/>
+    <mergeCell ref="BT38:BT39"/>
+    <mergeCell ref="BU38:BU39"/>
+    <mergeCell ref="BG38:BG39"/>
+    <mergeCell ref="AV38:AV39"/>
+    <mergeCell ref="U38:U39"/>
+    <mergeCell ref="BH38:BH39"/>
+    <mergeCell ref="BI38:BI39"/>
+    <mergeCell ref="BJ38:BJ39"/>
+    <mergeCell ref="T38:T39"/>
+    <mergeCell ref="AM38:AM39"/>
+    <mergeCell ref="AN38:AN39"/>
+    <mergeCell ref="AO38:AO39"/>
+    <mergeCell ref="AP38:AP39"/>
+    <mergeCell ref="AQ38:AQ39"/>
+    <mergeCell ref="AL38:AL39"/>
+    <mergeCell ref="BO38:BO39"/>
+    <mergeCell ref="AU38:AU39"/>
+    <mergeCell ref="BA38:BA39"/>
+    <mergeCell ref="BF38:BF39"/>
+    <mergeCell ref="BR38:BR39"/>
+    <mergeCell ref="BQ38:BQ39"/>
+    <mergeCell ref="BP38:BP39"/>
+    <mergeCell ref="BE38:BE39"/>
+    <mergeCell ref="BL38:BL39"/>
+    <mergeCell ref="BN25:BN26"/>
+    <mergeCell ref="BO25:BO26"/>
+    <mergeCell ref="BP25:BP26"/>
+    <mergeCell ref="BE25:BE26"/>
+    <mergeCell ref="BL25:BL26"/>
+    <mergeCell ref="BM25:BM26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="BI25:BI26"/>
+    <mergeCell ref="BJ25:BJ26"/>
+    <mergeCell ref="T25:T26"/>
+    <mergeCell ref="S25:S26"/>
+    <mergeCell ref="BK25:BK26"/>
+    <mergeCell ref="R25:R26"/>
+    <mergeCell ref="X25:X26"/>
+    <mergeCell ref="Y25:Y26"/>
+    <mergeCell ref="AA25:AA26"/>
+    <mergeCell ref="AM25:AM26"/>
+    <mergeCell ref="AN25:AN26"/>
+    <mergeCell ref="AO25:AO26"/>
+    <mergeCell ref="AK25:AK26"/>
+    <mergeCell ref="AH25:AH26"/>
+    <mergeCell ref="AT25:AT26"/>
+    <mergeCell ref="AY11:AY12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="AE11:AE12"/>
+    <mergeCell ref="BS25:BS26"/>
+    <mergeCell ref="AU25:AU26"/>
+    <mergeCell ref="BA25:BA26"/>
+    <mergeCell ref="V38:V39"/>
+    <mergeCell ref="X38:X39"/>
+    <mergeCell ref="Y38:Y39"/>
+    <mergeCell ref="AA38:AA39"/>
+    <mergeCell ref="BR25:BR26"/>
+    <mergeCell ref="BQ25:BQ26"/>
+    <mergeCell ref="AS25:AS26"/>
+    <mergeCell ref="AW25:AW26"/>
+    <mergeCell ref="Z25:Z26"/>
+    <mergeCell ref="W25:W26"/>
+    <mergeCell ref="AX25:AX26"/>
+    <mergeCell ref="AG25:AG26"/>
+    <mergeCell ref="AD25:AD26"/>
+    <mergeCell ref="AC25:AC26"/>
+    <mergeCell ref="AE25:AE26"/>
+    <mergeCell ref="AB25:AB26"/>
+    <mergeCell ref="AJ25:AJ26"/>
+    <mergeCell ref="BB25:BB26"/>
+    <mergeCell ref="BU25:BU26"/>
+    <mergeCell ref="AL25:AL26"/>
+    <mergeCell ref="AV25:AV26"/>
+    <mergeCell ref="U25:U26"/>
+    <mergeCell ref="AL11:AL12"/>
+    <mergeCell ref="AQ11:AQ12"/>
+    <mergeCell ref="AP11:AP12"/>
+    <mergeCell ref="AO11:AO12"/>
+    <mergeCell ref="AN11:AN12"/>
+    <mergeCell ref="BS11:BS12"/>
+    <mergeCell ref="BT11:BT12"/>
+    <mergeCell ref="BF25:BF26"/>
+    <mergeCell ref="AY25:AY26"/>
+    <mergeCell ref="AZ25:AZ26"/>
+    <mergeCell ref="AI25:AI26"/>
+    <mergeCell ref="BC25:BC26"/>
+    <mergeCell ref="BD25:BD26"/>
+    <mergeCell ref="AR25:AR26"/>
+    <mergeCell ref="BN11:BN12"/>
+    <mergeCell ref="BB11:BB12"/>
+    <mergeCell ref="BM11:BM12"/>
+    <mergeCell ref="BL11:BL12"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="Z11:Z12"/>
+    <mergeCell ref="BU11:BU12"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="AV11:AV12"/>
+    <mergeCell ref="BK11:BK12"/>
+    <mergeCell ref="AM11:AM12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="AC11:AC12"/>
+    <mergeCell ref="AD11:AD12"/>
+    <mergeCell ref="AG11:AG12"/>
+    <mergeCell ref="AF11:AF12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="BP11:BP12"/>
+    <mergeCell ref="BQ11:BQ12"/>
+    <mergeCell ref="BR11:BR12"/>
+    <mergeCell ref="BF11:BF12"/>
+    <mergeCell ref="BA11:BA12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="AW11:AW12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="BT25:BT26"/>
+    <mergeCell ref="V11:V12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="BH25:BH26"/>
+    <mergeCell ref="AP25:AP26"/>
+    <mergeCell ref="AQ25:AQ26"/>
+    <mergeCell ref="AK11:AK12"/>
+    <mergeCell ref="V25:V26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="Q25:Q26"/>
+    <mergeCell ref="AF25:AF26"/>
+    <mergeCell ref="BG25:BG26"/>
+    <mergeCell ref="AB11:AB12"/>
+    <mergeCell ref="AJ11:AJ12"/>
+    <mergeCell ref="BH11:BH12"/>
+    <mergeCell ref="BI11:BI12"/>
+    <mergeCell ref="AH11:AH12"/>
+    <mergeCell ref="BO11:BO12"/>
+    <mergeCell ref="Y11:Y12"/>
+    <mergeCell ref="BE11:BE12"/>
+    <mergeCell ref="AI11:AI12"/>
+    <mergeCell ref="AS11:AS12"/>
+    <mergeCell ref="AR11:AR12"/>
     <mergeCell ref="BJ11:BJ12"/>
     <mergeCell ref="T11:T12"/>
     <mergeCell ref="F11:F12"/>
@@ -15278,262 +15534,6 @@
     <mergeCell ref="AA11:AA12"/>
     <mergeCell ref="BG11:BG12"/>
     <mergeCell ref="AZ11:AZ12"/>
-    <mergeCell ref="BT25:BT26"/>
-    <mergeCell ref="V11:V12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="BH25:BH26"/>
-    <mergeCell ref="AP25:AP26"/>
-    <mergeCell ref="AQ25:AQ26"/>
-    <mergeCell ref="AK11:AK12"/>
-    <mergeCell ref="V25:V26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="Q25:Q26"/>
-    <mergeCell ref="AF25:AF26"/>
-    <mergeCell ref="BG25:BG26"/>
-    <mergeCell ref="AB11:AB12"/>
-    <mergeCell ref="AJ11:AJ12"/>
-    <mergeCell ref="BH11:BH12"/>
-    <mergeCell ref="BI11:BI12"/>
-    <mergeCell ref="AH11:AH12"/>
-    <mergeCell ref="BO11:BO12"/>
-    <mergeCell ref="Y11:Y12"/>
-    <mergeCell ref="BE11:BE12"/>
-    <mergeCell ref="AI11:AI12"/>
-    <mergeCell ref="AS11:AS12"/>
-    <mergeCell ref="AR11:AR12"/>
-    <mergeCell ref="BU11:BU12"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="AV11:AV12"/>
-    <mergeCell ref="BK11:BK12"/>
-    <mergeCell ref="AM11:AM12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="AC11:AC12"/>
-    <mergeCell ref="AD11:AD12"/>
-    <mergeCell ref="AG11:AG12"/>
-    <mergeCell ref="AF11:AF12"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="BP11:BP12"/>
-    <mergeCell ref="BQ11:BQ12"/>
-    <mergeCell ref="BR11:BR12"/>
-    <mergeCell ref="BF11:BF12"/>
-    <mergeCell ref="BA11:BA12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="AW11:AW12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="BU25:BU26"/>
-    <mergeCell ref="AL25:AL26"/>
-    <mergeCell ref="AV25:AV26"/>
-    <mergeCell ref="U25:U26"/>
-    <mergeCell ref="AL11:AL12"/>
-    <mergeCell ref="AQ11:AQ12"/>
-    <mergeCell ref="AP11:AP12"/>
-    <mergeCell ref="AO11:AO12"/>
-    <mergeCell ref="AN11:AN12"/>
-    <mergeCell ref="BS11:BS12"/>
-    <mergeCell ref="BT11:BT12"/>
-    <mergeCell ref="BF25:BF26"/>
-    <mergeCell ref="AY25:AY26"/>
-    <mergeCell ref="AZ25:AZ26"/>
-    <mergeCell ref="AI25:AI26"/>
-    <mergeCell ref="BC25:BC26"/>
-    <mergeCell ref="BD25:BD26"/>
-    <mergeCell ref="AR25:AR26"/>
-    <mergeCell ref="BN11:BN12"/>
-    <mergeCell ref="BB11:BB12"/>
-    <mergeCell ref="BM11:BM12"/>
-    <mergeCell ref="BL11:BL12"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="Z11:Z12"/>
-    <mergeCell ref="AY11:AY12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="AE11:AE12"/>
-    <mergeCell ref="BS25:BS26"/>
-    <mergeCell ref="AU25:AU26"/>
-    <mergeCell ref="BA25:BA26"/>
-    <mergeCell ref="V38:V39"/>
-    <mergeCell ref="X38:X39"/>
-    <mergeCell ref="Y38:Y39"/>
-    <mergeCell ref="AA38:AA39"/>
-    <mergeCell ref="BR25:BR26"/>
-    <mergeCell ref="BQ25:BQ26"/>
-    <mergeCell ref="AS25:AS26"/>
-    <mergeCell ref="AW25:AW26"/>
-    <mergeCell ref="Z25:Z26"/>
-    <mergeCell ref="W25:W26"/>
-    <mergeCell ref="AX25:AX26"/>
-    <mergeCell ref="AG25:AG26"/>
-    <mergeCell ref="AD25:AD26"/>
-    <mergeCell ref="AC25:AC26"/>
-    <mergeCell ref="AE25:AE26"/>
-    <mergeCell ref="AB25:AB26"/>
-    <mergeCell ref="AJ25:AJ26"/>
-    <mergeCell ref="BB25:BB26"/>
-    <mergeCell ref="BN25:BN26"/>
-    <mergeCell ref="BO25:BO26"/>
-    <mergeCell ref="BP25:BP26"/>
-    <mergeCell ref="BE25:BE26"/>
-    <mergeCell ref="BL25:BL26"/>
-    <mergeCell ref="BM25:BM26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="BI25:BI26"/>
-    <mergeCell ref="BJ25:BJ26"/>
-    <mergeCell ref="T25:T26"/>
-    <mergeCell ref="S25:S26"/>
-    <mergeCell ref="BK25:BK26"/>
-    <mergeCell ref="R25:R26"/>
-    <mergeCell ref="X25:X26"/>
-    <mergeCell ref="Y25:Y26"/>
-    <mergeCell ref="AA25:AA26"/>
-    <mergeCell ref="AM25:AM26"/>
-    <mergeCell ref="AN25:AN26"/>
-    <mergeCell ref="AO25:AO26"/>
-    <mergeCell ref="AK25:AK26"/>
-    <mergeCell ref="AH25:AH26"/>
-    <mergeCell ref="AT25:AT26"/>
-    <mergeCell ref="BT38:BT39"/>
-    <mergeCell ref="BU38:BU39"/>
-    <mergeCell ref="BG38:BG39"/>
-    <mergeCell ref="AV38:AV39"/>
-    <mergeCell ref="U38:U39"/>
-    <mergeCell ref="BH38:BH39"/>
-    <mergeCell ref="BI38:BI39"/>
-    <mergeCell ref="BJ38:BJ39"/>
-    <mergeCell ref="T38:T39"/>
-    <mergeCell ref="AM38:AM39"/>
-    <mergeCell ref="AN38:AN39"/>
-    <mergeCell ref="AO38:AO39"/>
-    <mergeCell ref="AP38:AP39"/>
-    <mergeCell ref="AQ38:AQ39"/>
-    <mergeCell ref="AL38:AL39"/>
-    <mergeCell ref="BO38:BO39"/>
-    <mergeCell ref="AU38:AU39"/>
-    <mergeCell ref="BA38:BA39"/>
-    <mergeCell ref="BF38:BF39"/>
-    <mergeCell ref="BR38:BR39"/>
-    <mergeCell ref="BQ38:BQ39"/>
-    <mergeCell ref="BP38:BP39"/>
-    <mergeCell ref="BE38:BE39"/>
-    <mergeCell ref="BL38:BL39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="S38:S39"/>
-    <mergeCell ref="BK38:BK39"/>
-    <mergeCell ref="BS38:BS39"/>
-    <mergeCell ref="P38:P39"/>
-    <mergeCell ref="Q38:Q39"/>
-    <mergeCell ref="AF38:AF39"/>
-    <mergeCell ref="AG38:AG39"/>
-    <mergeCell ref="AD38:AD39"/>
-    <mergeCell ref="AC38:AC39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="O38:O39"/>
-    <mergeCell ref="BM38:BM39"/>
-    <mergeCell ref="BB38:BB39"/>
-    <mergeCell ref="BN38:BN39"/>
-    <mergeCell ref="W38:W39"/>
-    <mergeCell ref="R38:R39"/>
-    <mergeCell ref="AX38:AX39"/>
-    <mergeCell ref="AY38:AY39"/>
-    <mergeCell ref="AZ38:AZ39"/>
-    <mergeCell ref="AT38:AT39"/>
-    <mergeCell ref="BC38:BC39"/>
-    <mergeCell ref="BD38:BD39"/>
-    <mergeCell ref="AR38:AR39"/>
-    <mergeCell ref="AS38:AS39"/>
-    <mergeCell ref="AW38:AW39"/>
-    <mergeCell ref="Z38:Z39"/>
-    <mergeCell ref="AE38:AE39"/>
-    <mergeCell ref="AB38:AB39"/>
-    <mergeCell ref="AJ38:AJ39"/>
-    <mergeCell ref="AK38:AK39"/>
-    <mergeCell ref="AH38:AH39"/>
-    <mergeCell ref="AI38:AI39"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="H52:H53"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="J52:J53"/>
-    <mergeCell ref="K52:K53"/>
-    <mergeCell ref="L52:L53"/>
-    <mergeCell ref="R52:R53"/>
-    <mergeCell ref="AX52:AX53"/>
-    <mergeCell ref="O52:O53"/>
-    <mergeCell ref="P52:P53"/>
-    <mergeCell ref="Q52:Q53"/>
-    <mergeCell ref="AF52:AF53"/>
-    <mergeCell ref="M52:M53"/>
-    <mergeCell ref="N52:N53"/>
-    <mergeCell ref="AL52:AL53"/>
-    <mergeCell ref="AV52:AV53"/>
-    <mergeCell ref="U52:U53"/>
-    <mergeCell ref="AO52:AO53"/>
-    <mergeCell ref="AP52:AP53"/>
-    <mergeCell ref="AQ52:AQ53"/>
-    <mergeCell ref="Y52:Y53"/>
-    <mergeCell ref="AA52:AA53"/>
-    <mergeCell ref="AM52:AM53"/>
-    <mergeCell ref="AN52:AN53"/>
-    <mergeCell ref="Z52:Z53"/>
-    <mergeCell ref="BS52:BS53"/>
-    <mergeCell ref="BT52:BT53"/>
-    <mergeCell ref="BU52:BU53"/>
-    <mergeCell ref="AW52:AW53"/>
-    <mergeCell ref="AG52:AG53"/>
-    <mergeCell ref="AD52:AD53"/>
-    <mergeCell ref="AC52:AC53"/>
-    <mergeCell ref="AE52:AE53"/>
-    <mergeCell ref="AB52:AB53"/>
-    <mergeCell ref="AJ52:AJ53"/>
-    <mergeCell ref="AK52:AK53"/>
-    <mergeCell ref="AH52:AH53"/>
-    <mergeCell ref="BR52:BR53"/>
-    <mergeCell ref="BQ52:BQ53"/>
-    <mergeCell ref="BP52:BP53"/>
-    <mergeCell ref="BE52:BE53"/>
-    <mergeCell ref="BL52:BL53"/>
-    <mergeCell ref="BM52:BM53"/>
-    <mergeCell ref="AS52:AS53"/>
-    <mergeCell ref="BI52:BI53"/>
-    <mergeCell ref="BJ52:BJ53"/>
-    <mergeCell ref="BK52:BK53"/>
-    <mergeCell ref="BB52:BB53"/>
-    <mergeCell ref="BN52:BN53"/>
-    <mergeCell ref="BO52:BO53"/>
-    <mergeCell ref="T52:T53"/>
-    <mergeCell ref="S52:S53"/>
-    <mergeCell ref="V52:V53"/>
-    <mergeCell ref="X52:X53"/>
-    <mergeCell ref="AT52:AT53"/>
-    <mergeCell ref="AU52:AU53"/>
-    <mergeCell ref="BA52:BA53"/>
-    <mergeCell ref="BF52:BF53"/>
-    <mergeCell ref="AY52:AY53"/>
-    <mergeCell ref="AZ52:AZ53"/>
-    <mergeCell ref="AI52:AI53"/>
-    <mergeCell ref="BC52:BC53"/>
-    <mergeCell ref="BD52:BD53"/>
-    <mergeCell ref="AR52:AR53"/>
-    <mergeCell ref="BG52:BG53"/>
-    <mergeCell ref="BH52:BH53"/>
-    <mergeCell ref="W52:W53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
@@ -15575,8 +15575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:O54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15787,7 +15787,7 @@
         <v>92</v>
       </c>
       <c r="L31" s="63" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="M31" s="63" t="s">
         <v>35</v>

</xml_diff>